<commit_message>
adding igus rail back in
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17060" yWindow="460" windowWidth="21420" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="12180" yWindow="460" windowWidth="21420" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tom" sheetId="3" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>